<commit_message>
add test for bank account in practice 2
</commit_message>
<xml_diff>
--- a/TestCases_xlsx/TestCases_practice_01.xlsx
+++ b/TestCases_xlsx/TestCases_practice_01.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\PycharmProjects\module_4_testing\TestCases_xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337961FA-6B8D-4CAF-9FA1-CF3CBE71D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Лист2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Лист3" sheetId="3" r:id="rId6"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -624,29 +633,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="d.m"/>
-    <numFmt numFmtId="165" formatCode="d.m."/>
+    <numFmt numFmtId="164" formatCode="d\.m"/>
+    <numFmt numFmtId="165" formatCode="d\.m\."/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -656,7 +668,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -666,79 +678,60 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -928,75 +921,80 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="B2:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="12.0"/>
-    <col customWidth="1" min="3" max="3" width="28.13"/>
-    <col customWidth="1" min="4" max="4" width="25.38"/>
-    <col customWidth="1" min="5" max="5" width="20.25"/>
-    <col customWidth="1" min="6" max="6" width="22.5"/>
-    <col customWidth="1" min="7" max="7" width="18.38"/>
-    <col customWidth="1" min="8" max="8" width="18.75"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1022,66 +1020,66 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="G17" s="3">
+        <v>7</v>
+      </c>
+      <c r="H17" s="3">
+        <v>7</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="6">
-        <v>45480.0</v>
-      </c>
-      <c r="H18" s="6">
-        <v>45480.0</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="5" t="s">
+      <c r="G18" s="5">
+        <v>45480</v>
+      </c>
+      <c r="H18" s="5">
+        <v>45480</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1091,29 +1089,29 @@
         <v>29</v>
       </c>
       <c r="G19" s="1">
-        <v>-13.0</v>
+        <v>-13</v>
       </c>
       <c r="H19" s="1">
-        <v>-13.0</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="5" t="s">
+        <v>-13</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -1122,155 +1120,155 @@
       <c r="H20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="5" t="s">
+      <c r="I20" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="5" t="s">
+      <c r="I21" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="5" t="s">
+      <c r="I22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="5" t="s">
+      <c r="I23" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="H25" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="5" t="s">
+      <c r="G25" s="4">
+        <v>2</v>
+      </c>
+      <c r="H25" s="4">
+        <v>2</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="5">
-        <v>-2.0</v>
-      </c>
-      <c r="H26" s="5">
-        <v>-2.0</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="5" t="s">
+      <c r="G26" s="4">
+        <v>-2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>-2</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1282,24 +1280,24 @@
       <c r="F27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="10">
-        <v>45325.0</v>
-      </c>
-      <c r="H27" s="10">
-        <v>45325.0</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="5" t="s">
+      <c r="G27" s="8">
+        <v>45325</v>
+      </c>
+      <c r="H27" s="8">
+        <v>45325</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -1309,20 +1307,20 @@
         <v>62</v>
       </c>
       <c r="G28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H28" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1337,18 +1335,18 @@
       <c r="G29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="I29" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1363,21 +1361,21 @@
       <c r="G30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31">
+      <c r="I30" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1390,20 +1388,20 @@
         <v>20</v>
       </c>
       <c r="G32" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="H32" s="1">
-        <v>50.0</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>50</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1421,15 +1419,15 @@
       <c r="H33" s="1">
         <v>13.75</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34">
+      <c r="I33" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -1442,20 +1440,20 @@
         <v>72</v>
       </c>
       <c r="G34" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="H34" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>25</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1473,15 +1471,15 @@
       <c r="H35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I35" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36">
+      <c r="I35" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -1499,15 +1497,15 @@
       <c r="H36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37">
+      <c r="I36" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1520,20 +1518,20 @@
         <v>81</v>
       </c>
       <c r="G37" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="H37" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>10</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -1551,15 +1549,16 @@
       <c r="H38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40">
+      <c r="I38" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -1572,20 +1571,20 @@
         <v>20</v>
       </c>
       <c r="G40" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H40" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>2</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -1603,15 +1602,15 @@
       <c r="H41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42">
+      <c r="I41" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -1633,11 +1632,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -1650,20 +1649,20 @@
         <v>102</v>
       </c>
       <c r="G43" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H43" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>5</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -1676,78 +1675,80 @@
         <v>105</v>
       </c>
       <c r="G44" s="1">
-        <v>-2.0</v>
+        <v>-2</v>
       </c>
       <c r="H44" s="1">
-        <v>-2.0</v>
-      </c>
-      <c r="I44" s="5" t="s">
+        <v>-2</v>
+      </c>
+      <c r="I44" s="4" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="9.0"/>
-    <col customWidth="1" min="3" max="3" width="26.25"/>
-    <col customWidth="1" min="4" max="4" width="17.63"/>
-    <col customWidth="1" min="5" max="5" width="19.25"/>
-    <col customWidth="1" min="6" max="6" width="20.75"/>
-    <col customWidth="1" min="7" max="7" width="18.38"/>
-    <col customWidth="1" min="8" max="8" width="20.88"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1773,150 +1774,150 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>112</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>115</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G18" s="11">
-        <v>45401.0</v>
-      </c>
-      <c r="H18" s="11">
-        <v>45401.0</v>
+      <c r="G18" s="9">
+        <v>45401</v>
+      </c>
+      <c r="H18" s="9">
+        <v>45401</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>118</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>120</v>
       </c>
       <c r="G19" s="1">
-        <v>-23.0</v>
+        <v>-23</v>
       </c>
       <c r="H19" s="1">
-        <v>-23.0</v>
+        <v>-23</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G20" s="1">
-        <v>-3.0</v>
+        <v>-3</v>
       </c>
       <c r="H20" s="1">
-        <v>-3.0</v>
+        <v>-3</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G21" s="11">
-        <v>45543.0</v>
-      </c>
-      <c r="H21" s="11">
-        <v>45543.0</v>
+      <c r="G21" s="9">
+        <v>45543</v>
+      </c>
+      <c r="H21" s="9">
+        <v>45543</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>128</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>130</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1929,20 +1930,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>131</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>133</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -1955,20 +1956,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -1981,46 +1982,46 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>141</v>
       </c>
       <c r="G25" s="1">
-        <v>1.24975E7</v>
+        <v>12497500</v>
       </c>
       <c r="H25" s="1">
-        <v>1.24975E7</v>
+        <v>12497500</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>143</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>145</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -2033,54 +2034,54 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27">
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="F27" s="9"/>
+    <row r="27" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="F27" s="4"/>
       <c r="I27" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>112</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G28" s="1">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="H28" s="1">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>115</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>117</v>
       </c>
       <c r="G29" s="1">
@@ -2093,98 +2094,98 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>118</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>120</v>
       </c>
       <c r="G30" s="1">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="H30" s="1">
-        <v>-960.0</v>
+        <v>-960</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G31" s="12">
-        <v>-1620.0</v>
-      </c>
-      <c r="H31" s="12">
-        <v>-1620.0</v>
+      <c r="G31" s="10">
+        <v>-1620</v>
+      </c>
+      <c r="H31" s="10">
+        <v>-1620</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="11">
         <v>11647.545</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="12">
         <v>11647.545</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>128</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>130</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -2197,20 +2198,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>131</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>133</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -2223,20 +2224,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G35" s="1" t="s">
@@ -2249,40 +2250,40 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>141</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>143</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>145</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -2295,155 +2296,155 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="I38" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>112</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G39" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>115</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="4" t="s">
         <v>117</v>
       </c>
       <c r="G40" s="1">
-        <v>4.85</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H40" s="1">
-        <v>4.85</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>118</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>120</v>
       </c>
       <c r="G41" s="1">
-        <v>-4.6</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="H41" s="1">
-        <v>-4.6</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G42" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="H42" s="12">
-        <v>2.0</v>
+      <c r="G42" s="10">
+        <v>2</v>
+      </c>
+      <c r="H42" s="10">
+        <v>2</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="11">
         <v>1.78</v>
       </c>
-      <c r="H43" s="13">
+      <c r="H43" s="11">
         <v>1.78</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>128</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="4" t="s">
         <v>130</v>
       </c>
       <c r="G44" s="1" t="s">
@@ -2456,20 +2457,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>131</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="4" t="s">
         <v>133</v>
       </c>
       <c r="G45" s="1" t="s">
@@ -2482,20 +2483,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G46" s="1" t="s">
@@ -2508,40 +2509,40 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>141</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="4" t="s">
         <v>143</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>145</v>
       </c>
       <c r="G48" s="1" t="s">
@@ -2555,54 +2556,57 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="19.5"/>
-    <col customWidth="1" min="4" max="4" width="23.13"/>
-    <col customWidth="1" min="5" max="5" width="16.0"/>
-    <col customWidth="1" min="6" max="6" width="17.0"/>
-    <col customWidth="1" min="7" max="7" width="21.13"/>
-    <col customWidth="1" min="8" max="8" width="18.75"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
@@ -2628,321 +2632,321 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>167</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="19">
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20">
+    <row r="19" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G20" s="1">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G21" s="1">
-        <v>66.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>178</v>
       </c>
       <c r="G23" s="1">
-        <v>99.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>182</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>182</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>192</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>192</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>192</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>192</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>182</v>
       </c>
       <c r="G32" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34">
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35">
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36">
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37">
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38">
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>